<commit_message>
Mark cells to start reading from at the time of worksheet construction
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/empty-sheets.xlsx
+++ b/tests/testthat/sheets/empty-sheets.xlsx
@@ -30,10 +30,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>X1</t>
+    <t>var1</t>
   </si>
   <si>
-    <t>X2</t>
+    <t>var2</t>
   </si>
 </sst>
 </file>
@@ -363,7 +363,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>